<commit_message>
updates to entries which consent was not given initially
</commit_message>
<xml_diff>
--- a/The Sigma Awards 2023 Shortlist (full projects data).xlsx
+++ b/The Sigma Awards 2023 Shortlist (full projects data).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuangkeng/Documents/mygithub/shortlist-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89DE3E9-3062-524C-9FAA-9460313F17DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0E10C2-8CAE-164F-BD2A-5D0A475D060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="-19620" windowWidth="27460" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27400" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="995">
   <si>
     <t>Country</t>
   </si>
@@ -624,9 +624,6 @@
 It combined sophisticated data mining techniques with meticulous research and shoe-leather reporting to examine, in unprecedented detail, the money flowing from the gambling industry into the political system.</t>
   </si>
   <si>
-    <t>The applicant did not give consent to publish parts of the application.</t>
-  </si>
-  <si>
     <t>https://www.abc.net.au/news/2022-05-10/gambling-industry-political-donations-to-states-and-territories/100988954</t>
   </si>
   <si>
@@ -785,28 +782,6 @@
   </si>
   <si>
     <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Reporter.lu (Luxembourg, in German).
-Meduza (Russia, in Russian),
-Le Monde (France, in French),
-Der Spiegel (Germany, in German),
-Profil (Austria, in German),
-Investigace.cz (Czech Republic, in Czech),
-Siena.lt (Lithuania, in Lithuanian),
-Eesti Ekspress (Estonia, in Estonian),
-The Guardian (U.K., in English),
-Information.dk (Denmark, in Danish),
-FTM (The Netherlands, in Dutch),
-Infolibre (Spain, in Spanish),
-Tijd (Belgium, in Flemish),
-Tamedia (Switzerland, in German),
-Tamedia (Switzerland, in French),
-Dagbladet Information (Denmark, in Danish),
-NDR/WDR (Germany, in German),
-IRPI (Italy, in Italian),
-YLE (Finland, in Finnish) and
-Inside Story (Greece, in Greek).</t>
   </si>
   <si>
     <t>Mysterious Group of Companies Tied to Bank Rossiya Unites Billions of Dollars in Assets Connected to Vladimir Putin</t>
@@ -1922,9 +1897,6 @@
   </si>
   <si>
     <t>http://sigmaawards.org/wp-content/uploads/2023/02/sigma2023-030.jpg</t>
-  </si>
-  <si>
-    <t>CCIJ, OpenUp, West Cape News</t>
   </si>
   <si>
     <t>Rivers of Sewage</t>
@@ -3520,26 +3492,6 @@
     <t>Yao-Hua Law</t>
   </si>
   <si>
-    <t>I have been a science and environment journalist in Malaysia since 2014. I have mostly reported on ecology and public health for top science magazines, including a narrative feature on snakebite health burden in Indonesia that won the One World Media Award in 2020. 
-In 2019, I co-founded Macaranga, an environmental journalism portal, to fill a gap in in-depth, data-driven and analytical environmental reporting in the country. When our reader interest survey singled out ‘deforestation’ as the top concern, I looked into the matter and started my years-long investigation on forest use and management in Peninsular Malaysia. At the time, no other Malaysian media provided accurate insights on the people or forces that drive forest use. Forestry data was often described as obscure and “confidential”, and the prevalent notion was that reporting on logging projects would trigger the wrath of tycoons, politicians, and royal families. 
-My stories for Macaranga, supported by the Pulitzer Center, showed otherwise. I saw how foreign media like Guardian, Bloomberg, and Economist were combining data, satellite imagery, visualisations and storytelling to produce impactful environmental reporting. I attempted a similar approach – though without a freedom of information act in Malaysia, data remain largely limited and scattered. Still, I have been able to sniff out several sources of data (resource centers in government department), learn to analyse satellite images and GIS data in QGIS, use free tools like Flourish, Pinpoint, and others to scrape websites. The stories I produced were very data-driven and data-supported, and successfully transported readers to the locality using maps and engaging writing. 
-It might have been a coincidence, but since Macaranga started publishing, other Malaysian media began to include more graphs, maps, and satellite images in their environmental reporting too. Well, I am one of several people training journalists in Malaysia on data journalism and environmental reporting. 
-In 2022, my stories for Macaranga won Malaysia’s top journalism award – the Malaysian Press Institute Award Gold Prize for Excellence in Environmental Reporting. Macaranga had just turned 3 years old then. But the best news last year was that a company stopped their logging after I reported on them, and the Department of Environment initiated investigation on a royalty-associated company after I exposed that they had broke the law on an oil palm project.</t>
-  </si>
-  <si>
-    <t>I am the sole reporter and I made almost all of the elements presented in the stories. These projects investigated unsustainable use of forests in Peninsular Malaysia, and exposed systemic failures, illegal activity, or projects that hurt the state and communities but benefit the shareholders.
-In “Forest Plantations in Reserves”, I showed that the governments’ forest plantation efforts have destroyed huge tracts of forests without achieving delivering any goals. Forest plantations are monoculture tree farms, and were meant to provide a sustainable timber supply. But I showed that governments only approved plantations inside reserves, and that two-thirds of the 185,000 ha cleared for plantations had been abandoned. Furthermore, genuine planters are struggling with their businesses and refuse to harvest timber as scheduled. 
-I analysed more than 40 years of forest plantation documents – government reports, conference papers, manuals, and scientific studies. I sought maps to check if and where plantations were destroying good forests. I combed through company financial statements and EIA reports of projects. I persuaded loggers and planters to explain the specifics of their projects; got government officers to confess that their data fails to reflect reality; and spoke with communities affected by forest plantations.
-The work required data that is distributed without clear organisation across several government agencies. I had to go to these agencies, daily for weeks to comb their shelves. To convince loggers and planters, I spent days roaming in town. 
-A month before my publication, the government suddenly announced a halt on new forest plantation projects. My findings were used in a debate in state legislative assembly. And in the year after publication, as forest plantations hit the news often, journalists and policymakers refer to my stories for background. 
-For “Cutting Chini-Bera Forests…”, I revealed how the state government and Department of Environment have approved an oil palm project doomed to fail. That’s because the project had and will clear natural forests, which disqualifies it from mandatory sustainability certification in Malaysia. The forests there houses tigers, elephants, and hornbills. The site also houses two indigenous villages, some of whom claim they were tricked by the developer into signing letters of consent. 
-Digging into company documents and property ownership, I showed that the developer’s shareholder include royalty and a major Thai conglomerate that brands itself as a tiger defender in Thailand. I made accurate maps and gathered satellite images of the deforestation, and used the evidence to prod Malaysian oil palm regulators into responding: they denounced the project. 
-After publication, the developer didn’t exercise their rights to start logging. A major conservation group suspended its partnership with the Thai conglomerate. And lawyers for the indigenous villagers are using my stories and data to build their court case. 
-In the third project, “Drains Dug, Trees Cut, Now Let’s it Approved”, I exposed a developer for clearing forests and planting oil palm before it even submitted the mandatory environmental impact assessment (EIA). This was a risky story to report on because the Sultan of the state and his family own the developer and the land. The evidence and data I present must be extra solid.
-I extracted location, names, and dates of legal procedures out of the project’s EIA report. I used satellite images to identify progress of deforestation. Then I used a drone to snap images of the development. But the drone limited range meant I had to enter the plantations, posing as a birder, to get exact coordinates of the site’s border and see the palm saplings planted. I also spoke with workers and locals.
-The story prompted the Department of Environment to investigate the developer.</t>
-  </si>
-  <si>
     <t>https://www.macaranga.org/forest-plantations-in-reserves-quick-to-cut-slow-to-grow/</t>
   </si>
   <si>
@@ -3794,9 +3746,6 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=xOHRFIhF0Y8</t>
-  </si>
-  <si>
-    <t>El COnfidencial</t>
   </si>
   <si>
     <t>El Confidencial</t>
@@ -4125,6 +4074,122 @@
   <si>
     <t>Airstrips of Destruction in Brazil and Venezuela by the Pulitzer Center´s Rainforest Investigations Network (RIN) -</t>
   </si>
+  <si>
+    <t>I have been a science and environment journalist in Malaysia since 2014. I have mostly reported on ecology and public health for top science magazines, including a narrative feature on snakebite health burden in Indonesia that won the One World Media Award in 2020.
+In 2019, Wong Siew Lyn and I co-founded Macaranga, an environmental journalism portal, to fill a gap in in-depth, data-driven and analytical environmental reporting in the country. When our reader interest survey singled out ‘deforestation’ as the top concern, we looked into the matter and started my years-long investigation on forest use and management in Peninsular Malaysia. At the time, no other Malaysian media provided accurate insights on the people or forces that drive forest use. Forestry data was often described as obscure and “confidential”, and the prevalent notion was that reporting on logging projects would trigger the wrath of tycoons, politicians, and royal families.
+Our stories for Macaranga, supported by the Pulitzer Center, showed otherwise. I saw how foreign media like Guardian, Bloomberg, and Economist were combining data, satellite imagery, visualisations and storytelling to produce impactful environmental reporting. I attempted a similar approach – though without a freedom of information act in Malaysia, data remain largely limited and scattered. Still, I have been able to sniff out several sources of data (resource centers in government department), learn to analyse satellite images and GIS data in QGIS, use free tools like Flourish, Pinpoint, and others to scrape websites. With Siew Lyn
+as editor, we produced stories that were very data-driven and data-supported, and successfully transported readers to the locality using maps and engaging writing.
+It might have been a coincidence, but since Macaranga started publishing, other Malaysian media began to include more graphs, maps, and satellite images in their environmental reporting too. Well, we are some of several people training journalists in Malaysia on data journalism and environmental reporting.
+In 2022, my stories for Macaranga won Malaysia’s top journalism award – the Malaysian Press Institute Award Gold Prize for Excellence in Environmental Reporting. Macaranga had just turned 3 years old then. But the best news last year was that a company stopped their logging after we reported on them, and the Department of Environment initiated investigation on a royalty-associated company after we exposed that they had broke the law on an oil palm project.</t>
+  </si>
+  <si>
+    <t>I am the sole reporter and I made almost all of the elements presented in the stories. Wong
+Siew Lyn edited all the stories. These projects investigated unsustainable use of forests in Peninsular Malaysia, and exposed systemic failures, illegal activity, or projects that hurt the state and communities but benefit the shareholders.
+In ‚ÄúForest Plantations in Reserves‚Äù, I showed that the governments‚Äô forest plantation efforts have destroyed huge tracts of forests without achieving delivering any goals. Forest plantations are monoculture tree farms, and were meant to provide a sustainable timber supply. But I showed that governments only approved plantations inside reserves, and that two-thirds of the 185,000 ha cleared for plantations had been abandoned. Furthermore, genuine planters are struggling with their businesses and refuse to harvest timber as scheduled. 
+I analysed more than 40 years of forest plantation documents ‚Äì government reports, conference papers, manuals, and scientific studies. I sought maps to check if and where plantations were destroying good forests. I combed through company financial statements and EIA reports of projects. I persuaded loggers and planters to explain the specifics of their projects; got government officers to confess that their data fails to reflect reality; and spoke with communities affected by forest plantations.
+The work required data that is distributed without clear organisation across several government agencies. I had to go to these agencies, daily for weeks to comb their shelves. To convince loggers and planters, I spent days roaming in town. 
+A month before my publication, the government suddenly announced a halt on new forest plantation projects. My findings were used in a debate in state legislative assembly. And in the year after publication, as forest plantations hit the news often, journalists and policymakers refer to my stories for background. 
+For ‚ÄúCutting Chini-Bera Forests‚Ä¶‚Äù, I revealed how the state government and Department of Environment have approved an oil palm project doomed to fail. That‚Äôs because the project had and will clear natural forests, which disqualifies it from mandatory sustainability certification in Malaysia. The forests there houses tigers, elephants, and hornbills. The site also houses two indigenous villages, some of whom claim they were tricked by the developer into signing letters of consent. 
+Digging into company documents and property ownership, I showed that the developer‚Äôs shareholder include royalty and a major Thai conglomerate that brands itself as a tiger defender in Thailand. I made accurate maps and gathered satellite images of the deforestation, and used the evidence to prod Malaysian oil palm regulators into responding: they denounced the project. 
+After publication, the developer didn‚Äôt exercise their rights to start logging. A major conservation group suspended its partnership with the Thai conglomerate. And lawyers for the indigenous villagers are using my stories and data to build their court case. 
+In the third project, ‚ÄúDrains Dug, Trees Cut, Now Let‚Äôs it Approved‚Äù, I exposed a developer for clearing forests and planting oil palm before it even submitted the mandatory environmental impact assessment (EIA). This was a risky story to report on because the Sultan of the state and his family own the developer and the land. The evidence and data I present must be extra solid.
+I extracted location, names, and dates of legal procedures out of the project‚Äôs EIA report. I used satellite images to identify progress of deforestation. Then I used a drone to snap images of the development. But the drone limited range meant I had to enter the plantations, posing as a birder, to get exact coordinates of the site‚Äôs border and see the palm saplings planted. I also spoke with workers and locals.
+The story prompted the Department of Environment to investigate the developer.</t>
+  </si>
+  <si>
+    <t>CCIJ, OpenUp, West Cape News, GroundUp</t>
+  </si>
+  <si>
+    <t>OCCRP, Reporter.lu (Luxembourg, in German).
+Meduza (Russia, in Russian),
+Le Monde (France, in French),
+Der Spiegel (Germany, in German),
+Profil (Austria, in German),
+Investigace.cz (Czech Republic, in Czech),
+Siena.lt (Lithuania, in Lithuanian),
+Eesti Ekspress (Estonia, in Estonian),
+The Guardian (U.K., in English),
+Information.dk (Denmark, in Danish),
+FTM (The Netherlands, in Dutch),
+Infolibre (Spain, in Spanish),
+Tijd (Belgium, in Flemish),
+Tamedia (Switzerland, in German),
+Tamedia (Switzerland, in French),
+Dagbladet Information (Denmark, in Danish),
+NDR/WDR (Germany, in German),
+IRPI (Italy, in Italian),
+YLE (Finland, in Finnish) and
+Inside Story (Greece, in Greek).</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Following the release of this story:
+The city Department of Transportation announced plans to redesign streets outside schools in poor communities of color to make them safer.
+The governor of New York cited the story's findings when signing a bill to expand a school-zone speed camera program in New York City.
+The mayor of New York City and the city’s top transportation official said the city must do more to keep children safe from cars outside schools.
+Local lawmakers expressed outrage about the story’s findings and called on the city to do more to protect children from cars outside schools.</t>
+  </si>
+  <si>
+    <t>This story is built on an analysis of more than a dozen datasets and other data sources published by New York City, most on its open data portal. Using PostgreSQL, PostGIS, QGIS, and Excel, Coburn merged these disparate data sources into a novel database that listed every car crash near a New York City public school since July 2015—excluding the first 15 months of the pandemic, when city students were largely learning remotely—as well as information on the enrollment and demographics of each school. This yielded startling insights into the dangers that children face navigating city streets on their way to and from school every day.
+To begin, Coburn acquired and cleaned datasets on: car crashes in the city; the locations, enrollment and demographics of more than 1,000 city schools across six school years; and school calendars, which Coburn had to scrape from PDFs. He then wrote a 70-line Postgres query to join all this data into a single database. For every car crash in the city since July 2015, excluding the early pandemic period, the database indicates whether the crash occurred within 250 feet of a school, whether it occurred during student arrival and departure hours, and how many poor, non-white, and total students were enrolled in each school at the time.
+The database required extensive cleaning before it could be analyzed. For example, Coburn had to manually reclassify crashes that occurred near schools but posed no threat to pedestrians or cyclists, such as those on grade-separated highways. Finalizing the data took weeks.
+Once finished, this database led to previously unknown discoveries about the extent of traffic violence around schools, including that there are 57% more crashes and 25% more injuries per mile on school streets than other city streets at 8 a.m. on school days, and that injury rates from car crashes are 43% higher outside majority Black or brown schools than majority-white schools.
+Coburn also created interactive maps for the story using Tableau.</t>
+  </si>
+  <si>
+    <t>New York City agencies were hostile to Streetsblog’s efforts to examine the threat that cars pose to children outside city-run schools. The city departments of transportation and education declined to make any officials available for interviews or to answer many questions for the story. The Department of Education even kicked Streetsblog out of a press conference instead of answering basic questions about the dangers children face walking to and from city schools (link: https://nyc.streetsblog.org/2022/09/29/department-of-education-kicks-streetsblog-out-of-media-event-instead-of-answering-question-on-school-street-safety/).
+Streetsblog is a small non-profit newsroom. This was the largest project Streetsblog has even undertaken.</t>
+  </si>
+  <si>
+    <t>This story demonstrates that seemingly unrelated datasets can contain important, newsworthy stories when joined together. By looking at the nexus of traffic violence and education, Streetsblog uncovered previously unknown dangers that cars pose to children outside their schools.
+The story also shows how injustice can hide in even commonplace activities. Upon first glance, there may appear to be little of journalistic interest about the daily routine of children walking to and from school. Closer scrutiny showed the topic was beset by problems and inequities that deserved public attention.</t>
+  </si>
+  <si>
+    <t>"This exclusive series provided clear evidence of the monetary ties between the gambling industry and Australia’s political parties at a time of intense public scrutiny of the gambling sector’s links to money laundering and organised crime. 
+It renewed calls for greater transparency and accountability of Australia’s federal political donations laws and gave impetus to the introduction of two separate bills for political donations reform at the federal level."</t>
+  </si>
+  <si>
+    <t>"At the heart of the project is our gambling payments database, which brings together, for the first time, the political donations registers for every state and territory. 
+Our “master dataset” combined and then expanded on datasets used in previous research. We uncovered dozens of new gambling entities by undertaking forensic examination of company records, annual reports, media archives, financial statements, etc. and consulting extensively with researchers, gambling reform groups, and other experts. 
+Many of these individuals and organisations had been excluded from previous analyses because they own or operate other business or political interests alongside gambling ventures.
+From here, we built our database by: 
+1.Matching our gambling client list with 22 years of data and metadata scraped from the AEC Transparency Register. 
+2.Combing through hundreds of PDF scans of original disclosure forms on the AEC website, manually collecting additional payment details missed or excluded from the online database. 
+3.Matching the master list with records extracted from each of the seven state and territory political donations registers, some of which had to be collated by hand from PDFs.
+This data-driven approach allowed us to examine the interconnected money trails for hundreds of gambling-related donors, and to uncover vital clues about the pattern, timing and purpose of payments. The result is the most comprehensive and detailed record to date of payments made by the gambling industry to Australia’s political parties."</t>
+  </si>
+  <si>
+    <t>"Unlike most countries, Australia’s gambling industry extends far beyond lotteries and casinos. This is one of the reasons the industry’s political influence is so difficult to quantify. 
+Our project adopted a new approach to this problem, expanding on previous analyses to trace political payments from more than 370 gambling-related businesses and individuals over 22 years."</t>
+  </si>
+  <si>
+    <t>"This story demonstrates that you don't need perfect or complete data to produce a powerful data-driven investigation. 
+Our project was the first to analyse gambling donations in the political donations registers for every state and territory. While the incompleteness of these databases made this a frustrating exercise, it also demonstrated a key point: that Australia's system for ensuring transparency and accountability of political donations falls far short of this goal -- which is precisely why it deserves to be the focus of media investigation."</t>
+  </si>
+  <si>
+    <t>We haven't made any big discoveries in this article. The inequalities highlighted in this story were more or less known by everyone living in Brussels. We simply objectivised them, personalised the statistics and put them in context. The article is interactive and allow people to enter their address (70% of the reader did enter their information). In total 55k people have read the article which for Medor (small belgian indenpendant edition) is pretty high.</t>
+  </si>
+  <si>
+    <t>We have developed the article using Svelte (a javascript framework). The visuals are made in d3js and some of the maps uses MapboxJS. The data preparation consisting of the treatment of hundreds of public data sets has been done using ObservableHQ.</t>
+  </si>
+  <si>
+    <t>This work has only been possible thanks to subsidies provided by the "fond du journalisme". Whitout this help I don't think we could have done it. This work has was spead accross a full year. We have gone through hundreds of public datasets about Brussels.</t>
+  </si>
+  <si>
+    <t>Data journalism is unfortunatly not very present in the Belgian media. We hope this piece could convince them that there is an audiance for it and that they should explore what is possible on their end.</t>
+  </si>
+  <si>
+    <t>El Confidencial es un periódico español online fundado en 2001. Se trata de un medio de información generalista, con especial foco en la política, la economía y las finanzas. En su trayectoria, destaca por ser el primer medio español que decidió crear una sección de datos. Desde entonces, ha participado en investigaciones internacionales como los Panama Papers. Desde 2017 también forma parte de la primera red de periodismo de datos europea, la EDJNet.</t>
+  </si>
+  <si>
+    <t>Presentamos este portfolio de forma conjunta entre la sección de datos, formatos e internacional de El Confidencial. Este año, uno de los retos informativos ha sido cómo contar las cifras de la guerra entre Rusia y Ucrania. La falta de información fidedigna en muchos aspectos ha llevado a pensar en nuevas formas de contar el avance del conflicto, con los datos disponibles, pero mateniendo el rigor que caracteriza nuestro trabajo.
+El primer reto fue intentar medir el arranque del conflicto a partir de los datos de las bajas. Para ello, nos preguntamos cuántos cuántos rusos estaban muriendo en Ucrania, a solo un mes del inicio del conflicto. Las cifras eran muy diferentes dependiendo de la fuente, por lo que creamos una visualización que permitiera explicar todos los posibles escenarios. Con una estimación cauta, mosotramos cómo el principio de esta guerra estaba siendo "un desastre al ritmo de 20 afganistanes". A través de un formato especial, con infografía y vídeos, pusimos en contexto las cifras del comienzo de la guerra en cuanto a las bajas tanto humanas como materiales, en comparación con otros conflictos. 
+También al principio del conflicto, contamos cómo el conflicto se planteaba en un contexto de aislamiento de Rusia. Visualizamos en un formato especial qué paíse apoyaban a Putin y cuáles eran los posicionamientos internos de la población rusa. Como se ha hecho en otros medios de comunicación, en El Confidencial tambiénse ha llevado a cabo un gran esfuerzo por contar con mapas la evolución de la invasión.
+En mayo, hicimos un repaso de los diez principales datos que explicaban la guerra, con infografías, mapas y vídeos para contar desde la destrucciones de las ciudades hasta los envíos de armamento.
+Entre las publicaciones con mapas, destacamos un proyecto en el que dimensionamos a la escala española la invasión de Rusia a Ucrania, para acercar esta información a nuestro lector.</t>
+  </si>
 </sst>
 </file>
 
@@ -4133,7 +4198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4203,6 +4268,13 @@
       <color rgb="FF1155CC"/>
       <name val="Open Sans"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -4246,7 +4318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -4296,6 +4368,17 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4521,8 +4604,8 @@
   </sheetPr>
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4535,10 +4618,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>975</v>
-      </c>
-      <c r="B1" s="22"/>
+      <c r="A1" s="26" t="s">
+        <v>969</v>
+      </c>
+      <c r="B1" s="27"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -4563,10 +4646,10 @@
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="8"/>
@@ -4592,10 +4675,10 @@
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="8"/>
@@ -4621,13 +4704,13 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -4653,10 +4736,10 @@
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="12" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -4681,13 +4764,13 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -4713,10 +4796,10 @@
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="14" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -4741,13 +4824,13 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -4773,10 +4856,10 @@
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="15" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -4801,13 +4884,13 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -10869,7 +10952,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -10894,13 +10977,13 @@
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11915,8 +11998,8 @@
   </sheetPr>
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12526,46 +12609,46 @@
       <c r="I10" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>162</v>
+      <c r="J10" s="22" t="s">
+        <v>985</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>986</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>987</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>988</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O10" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="P10" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="V10" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>26</v>
@@ -12574,60 +12657,60 @@
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F11" s="2">
         <v>44580</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="V11" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>43</v>
@@ -12636,60 +12719,60 @@
         <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="2">
         <v>44648</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="V12" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>204</v>
+        <v>980</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>979</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -12698,49 +12781,49 @@
         <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F13" s="2">
         <v>44732</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="O13" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="P13" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="Q13" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="V13" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="W13" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>218</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>55</v>
@@ -12748,10 +12831,10 @@
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>26</v>
@@ -12760,64 +12843,64 @@
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F14" s="2">
         <v>44833</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="O14" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="P14" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="R14" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="S14" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="R14" s="3" t="s">
+      <c r="T14" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="U14" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="T14" s="3" t="s">
+      <c r="V14" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="W14" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12825,7 +12908,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
@@ -12834,64 +12917,64 @@
         <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F15" s="2">
         <v>44583</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="O15" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="P15" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="Q15" s="3" t="s">
+      <c r="S15" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="T15" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="S15" s="3" t="s">
+      <c r="U15" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="T15" s="3" t="s">
+      <c r="V15" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="U15" s="3" t="s">
+      <c r="W15" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -12899,7 +12982,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>26</v>
@@ -12908,72 +12991,72 @@
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F16" s="2">
         <v>44571</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O16" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="S16" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="R16" s="3" t="s">
+      <c r="T16" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="S16" s="3" t="s">
+      <c r="U16" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="T16" s="3" t="s">
+      <c r="V16" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="U16" s="3" t="s">
+      <c r="W16" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="X16" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>26</v>
@@ -12982,69 +13065,69 @@
         <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F17" s="2">
         <v>44678</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="O17" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="P17" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="R17" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="Q17" s="3" t="s">
+      <c r="S17" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="R17" s="3" t="s">
+      <c r="T17" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="S17" s="3" t="s">
+      <c r="V17" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="T17" s="3" t="s">
+      <c r="W17" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="X17" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
@@ -13053,55 +13136,55 @@
         <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F18" s="2">
         <v>44836</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="P18" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="Q18" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="R18" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="V18" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="R18" s="3" t="s">
+      <c r="W18" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13109,7 +13192,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>26</v>
@@ -13118,49 +13201,49 @@
         <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F19" s="2">
         <v>44788</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O19" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="V19" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="W19" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="X19" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="X19" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13168,7 +13251,7 @@
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>26</v>
@@ -13177,64 +13260,64 @@
         <v>27</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F20" s="2">
         <v>44636</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O20" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q20" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="R20" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="S20" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="R20" s="3" t="s">
+      <c r="T20" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="U20" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="T20" s="3" t="s">
+      <c r="V20" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="W20" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="X20" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13242,7 +13325,7 @@
         <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>26</v>
@@ -13251,57 +13334,57 @@
         <v>27</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F21" s="2">
         <v>44760</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O21" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="V21" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="W21" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="X21" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="X21" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>26</v>
@@ -13310,66 +13393,66 @@
         <v>27</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F22" s="2">
         <v>44894</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="O22" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="P22" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="R22" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="Q22" s="3" t="s">
+      <c r="S22" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="R22" s="3" t="s">
+      <c r="V22" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="S22" s="3" t="s">
+      <c r="W22" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>43</v>
@@ -13378,64 +13461,64 @@
         <v>27</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F23" s="2">
         <v>44924</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="N23" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="O23" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="P23" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="O23" s="3" t="s">
+      <c r="Q23" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="R23" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="Q23" s="3" t="s">
+      <c r="S23" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="R23" s="3" t="s">
+      <c r="T23" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="S23" s="3" t="s">
+      <c r="U23" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="T23" s="3" t="s">
+      <c r="V23" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="U23" s="3" t="s">
+      <c r="W23" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="V23" s="1" t="s">
+      <c r="X23" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="X23" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13443,7 +13526,7 @@
         <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>26</v>
@@ -13452,54 +13535,54 @@
         <v>27</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F24" s="2">
         <v>44720</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O24" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="W24" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="V24" s="1" t="s">
+      <c r="X24" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>43</v>
@@ -13508,46 +13591,46 @@
         <v>27</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F25" s="2">
         <v>44917</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O25" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="V25" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="W25" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="X25" s="4" t="s">
         <v>55</v>
@@ -13555,10 +13638,10 @@
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -13567,69 +13650,69 @@
         <v>27</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F26" s="2">
         <v>44679</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="O26" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="P26" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="R26" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="S26" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="T26" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="S26" s="3" t="s">
+      <c r="V26" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="T26" s="3" t="s">
+      <c r="W26" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="V26" s="1" t="s">
+      <c r="X26" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="X26" s="1" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>43</v>
@@ -13638,57 +13721,57 @@
         <v>27</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F27" s="2">
         <v>44914</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="O27" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="P27" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="V27" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="P27" s="3" t="s">
+      <c r="W27" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="V27" s="1" t="s">
+      <c r="X27" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="W27" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="X27" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>26</v>
@@ -13697,61 +13780,61 @@
         <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F28" s="2">
         <v>44660</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="O28" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="P28" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="Q28" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="R28" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="Q28" s="3" t="s">
+      <c r="S28" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="R28" s="3" t="s">
+      <c r="T28" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="S28" s="3" t="s">
+      <c r="V28" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="T28" s="3" t="s">
+      <c r="W28" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="V28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13759,7 +13842,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>483</v>
+        <v>978</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>26</v>
@@ -13768,64 +13851,64 @@
         <v>27</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F29" s="2">
         <v>44718</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O29" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="R29" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="S29" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="Q29" s="3" t="s">
+      <c r="T29" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="R29" s="3" t="s">
+      <c r="U29" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="S29" s="3" t="s">
+      <c r="V29" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="T29" s="3" t="s">
+      <c r="W29" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="U29" s="3" t="s">
+      <c r="X29" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="W29" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13833,7 +13916,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>26</v>
@@ -13842,72 +13925,72 @@
         <v>27</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F30" s="2">
         <v>44728</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>96</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>507</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="O30" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="P30" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="Q30" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="O30" s="3" t="s">
+      <c r="R30" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="P30" s="3" t="s">
+      <c r="S30" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="Q30" s="3" t="s">
+      <c r="T30" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="R30" s="3" t="s">
+      <c r="U30" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="S30" s="3" t="s">
+      <c r="V30" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="T30" s="3" t="s">
+      <c r="W30" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="U30" s="3" t="s">
+      <c r="X30" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="V30" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="X30" s="1" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>43</v>
@@ -13916,61 +13999,61 @@
         <v>27</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F31" s="2">
         <v>44623</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>530</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>150</v>
       </c>
       <c r="O31" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="R31" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="S31" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="T31" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="R31" s="3" t="s">
+      <c r="V31" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="W31" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="T31" s="3" t="s">
+      <c r="X31" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="V31" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="W31" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="X31" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13978,7 +14061,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>43</v>
@@ -13987,55 +14070,55 @@
         <v>27</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F32" s="2">
         <v>44574</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>548</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O32" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="R32" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="P32" s="3" t="s">
+      <c r="V32" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="Q32" s="3" t="s">
+      <c r="W32" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="R32" s="3" t="s">
+      <c r="X32" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="W32" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="X32" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14043,7 +14126,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
@@ -14052,64 +14135,64 @@
         <v>27</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="F33" s="2">
         <v>44880</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>564</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O33" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="R33" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="P33" s="3" t="s">
+      <c r="S33" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="Q33" s="3" t="s">
+      <c r="T33" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="R33" s="3" t="s">
+      <c r="U33" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="S33" s="3" t="s">
+      <c r="V33" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="T33" s="3" t="s">
+      <c r="W33" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="U33" s="3" t="s">
+      <c r="X33" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="V33" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="W33" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="X33" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14117,7 +14200,7 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>43</v>
@@ -14126,63 +14209,63 @@
         <v>27</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F34" s="2">
         <v>44853</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>583</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O34" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="R34" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="P34" s="3" t="s">
+      <c r="V34" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="Q34" s="3" t="s">
+      <c r="W34" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="R34" s="3" t="s">
+      <c r="X34" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="V34" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="W34" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="X34" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>43</v>
@@ -14191,66 +14274,66 @@
         <v>27</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F35" s="2">
         <v>44887</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="O35" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="P35" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="Q35" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="O35" s="3" t="s">
+      <c r="R35" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="P35" s="3" t="s">
+      <c r="S35" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="Q35" s="3" t="s">
+      <c r="V35" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="R35" s="3" t="s">
+      <c r="W35" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="S35" s="3" t="s">
+      <c r="X35" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="X35" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>26</v>
@@ -14259,54 +14342,54 @@
         <v>27</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="F36" s="2">
         <v>44852</v>
       </c>
       <c r="G36" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="O36" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="V36" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="W36" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="X36" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="X36" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>26</v>
@@ -14315,55 +14398,55 @@
         <v>27</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F37" s="2">
         <v>44755</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="O37" s="3" t="s">
         <v>632</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="P37" s="3" t="s">
         <v>633</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="Q37" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="R37" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="P37" s="3" t="s">
+      <c r="V37" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="Q37" s="3" t="s">
+      <c r="W37" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="R37" s="3" t="s">
+      <c r="X37" s="1" t="s">
         <v>638</v>
-      </c>
-      <c r="V37" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="W37" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="X37" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14371,7 +14454,7 @@
         <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>43</v>
@@ -14380,61 +14463,61 @@
         <v>27</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="F38" s="2">
         <v>44705</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>162</v>
+        <v>643</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>981</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>982</v>
+      </c>
+      <c r="L38" s="23" t="s">
+        <v>983</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>984</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O38" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="R38" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="P38" s="3" t="s">
+      <c r="S38" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="Q38" s="3" t="s">
+      <c r="T38" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="R38" s="3" t="s">
+      <c r="V38" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="S38" s="3" t="s">
+      <c r="W38" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="T38" s="3" t="s">
+      <c r="X38" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="V38" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="W38" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="X38" s="1" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14442,7 +14525,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>26</v>
@@ -14451,64 +14534,64 @@
         <v>27</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="F39" s="2">
         <v>44682</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>661</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>664</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O39" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="R39" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="P39" s="3" t="s">
+      <c r="S39" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="Q39" s="3" t="s">
+      <c r="T39" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="R39" s="3" t="s">
+      <c r="U39" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="S39" s="3" t="s">
+      <c r="V39" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="T39" s="3" t="s">
+      <c r="W39" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="U39" s="3" t="s">
+      <c r="X39" s="1" t="s">
         <v>671</v>
-      </c>
-      <c r="V39" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="W39" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="X39" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14516,7 +14599,7 @@
         <v>156</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>26</v>
@@ -14525,46 +14608,46 @@
         <v>27</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="F40" s="2">
         <v>44798</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>683</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O40" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="W40" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="P40" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="V40" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="W40" s="1" t="s">
-        <v>687</v>
       </c>
       <c r="X40" s="3" t="s">
         <v>55</v>
@@ -14572,10 +14655,10 @@
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>43</v>
@@ -14584,58 +14667,58 @@
         <v>27</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="F41" s="2">
         <v>44627</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="N41" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="O41" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="P41" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="Q41" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="N41" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="O41" s="3" t="s">
+      <c r="R41" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="P41" s="3" t="s">
+      <c r="S41" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="Q41" s="3" t="s">
+      <c r="V41" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="R41" s="3" t="s">
+      <c r="W41" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="S41" s="3" t="s">
+      <c r="X41" s="1" t="s">
         <v>701</v>
-      </c>
-      <c r="V41" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="W41" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="X41" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="42" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -14643,7 +14726,7 @@
         <v>140</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>26</v>
@@ -14652,54 +14735,54 @@
         <v>27</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="F42" s="2">
         <v>44712</v>
       </c>
       <c r="G42" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="J42" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>713</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>150</v>
       </c>
       <c r="O42" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="V42" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="W42" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="X42" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="W42" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="X42" s="1" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>43</v>
@@ -14708,54 +14791,54 @@
         <v>27</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="F43" s="2">
         <v>44715</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>989</v>
+      </c>
+      <c r="K43" s="22" t="s">
+        <v>990</v>
+      </c>
+      <c r="L43" s="22" t="s">
+        <v>991</v>
+      </c>
+      <c r="M43" s="22" t="s">
+        <v>992</v>
+      </c>
+      <c r="N43" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="O43" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="V43" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N43" s="1" t="s">
+      <c r="W43" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="O43" s="3" t="s">
+      <c r="X43" s="1" t="s">
         <v>725</v>
-      </c>
-      <c r="V43" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="W43" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="X43" s="1" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>26</v>
@@ -14764,49 +14847,49 @@
         <v>27</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="F44" s="2">
         <v>44656</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="O44" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="P44" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="V44" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="O44" s="3" t="s">
+      <c r="W44" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="P44" s="3" t="s">
+      <c r="X44" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="W44" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="X44" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -15006,8 +15089,8 @@
   </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15032,10 +15115,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -15062,21 +15145,21 @@
         <v>20</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>43</v>
@@ -15085,37 +15168,37 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>758</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>759</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>760</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15123,7 +15206,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>26</v>
@@ -15132,54 +15215,54 @@
         <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>766</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>767</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>768</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>771</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>772</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>773</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>774</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
@@ -15188,48 +15271,48 @@
         <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>778</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>779</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>780</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>781</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>783</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>785</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>787</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
@@ -15238,46 +15321,46 @@
         <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>792</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>793</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>794</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>795</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>796</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>797</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>798</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>799</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>800</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>801</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>802</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15285,7 +15368,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>26</v>
@@ -15294,42 +15377,42 @@
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>981</v>
+        <v>975</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>805</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>806</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="K6" s="3" t="s">
         <v>807</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>808</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>809</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>810</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>811</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>812</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>26</v>
@@ -15338,54 +15421,54 @@
         <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>817</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>820</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>822</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>826</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>827</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>828</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -15394,45 +15477,45 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="I8" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>834</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>837</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>838</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>839</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>43</v>
@@ -15441,34 +15524,34 @@
         <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="I9" s="3" t="s">
         <v>846</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="J9" s="3" t="s">
         <v>847</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="K9" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>849</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>851</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>852</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>853</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15476,7 +15559,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
@@ -15485,54 +15568,54 @@
         <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>861</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>863</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>865</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>866</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>867</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>43</v>
@@ -15541,25 +15624,25 @@
         <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>871</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>873</v>
+        <v>868</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>976</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>977</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15567,7 +15650,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
@@ -15576,51 +15659,51 @@
         <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>880</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>881</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>882</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>883</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>884</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>885</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>886</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>887</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>889</v>
+        <v>884</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -15629,28 +15712,28 @@
         <v>27</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>891</v>
+        <v>886</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15658,7 +15741,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>26</v>
@@ -15667,46 +15750,46 @@
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>901</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="O14" s="3" t="s">
         <v>902</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="P14" s="3" t="s">
         <v>903</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>904</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="R14" s="3" t="s">
         <v>905</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>906</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>907</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>908</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>909</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15714,7 +15797,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
@@ -15723,54 +15806,54 @@
         <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>915</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="O15" s="3" t="s">
         <v>916</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>917</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>918</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>919</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>920</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>921</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>922</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>923</v>
-      </c>
-      <c r="R15" s="3" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>43</v>
@@ -15779,34 +15862,34 @@
         <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>922</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>923</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>926</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="K16" s="3" t="s">
         <v>927</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="L16" s="3" t="s">
         <v>928</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="M16" s="3" t="s">
         <v>929</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>930</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>931</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>932</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>933</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>934</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15814,7 +15897,7 @@
         <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>26</v>
@@ -15823,36 +15906,36 @@
         <v>27</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>937</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>162</v>
+        <v>931</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>993</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>994</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>43</v>
@@ -15861,40 +15944,40 @@
         <v>27</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>943</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>944</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="M18" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="N18" s="3" t="s">
         <v>946</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="I18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>947</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="P18" s="3" t="s">
         <v>948</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>949</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>950</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>951</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>952</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>953</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>954</v>
       </c>
     </row>
   </sheetData>
@@ -16029,5 +16112,6 @@
     <hyperlink ref="P18" r:id="rId128" xr:uid="{00000000-0004-0000-0100-00007F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>